<commit_message>
use row iterator to get all active rows; add doc for build env and install dependencies
</commit_message>
<xml_diff>
--- a/test_excel.xlsx
+++ b/test_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/changl/excel_api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2A8310-84A5-624C-BFBF-95BE1181F2C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4DF41D-8FC6-4C4C-A75E-4F97890BEA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{FE8B6715-D06A-E049-99D2-C2B894523468}"/>
   </bookViews>
@@ -34,12 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>AUS</t>
   </si>
   <si>
     <t>USA</t>
+  </si>
+  <si>
+    <t>CHN</t>
   </si>
 </sst>
 </file>
@@ -403,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC477003-1363-674F-9921-AA81DF974A38}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -427,6 +430,11 @@
         <v>44197</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="AUS" tooltip="ISO 3166-1 alpha-3" display="https://en.wikipedia.org/wiki/ISO_3166-1_alpha-3 - AUS" xr:uid="{91F57B58-9420-B14B-9DB2-2C1975E96636}"/>

</xml_diff>

<commit_message>
add updated test file
</commit_message>
<xml_diff>
--- a/test_excel.xlsx
+++ b/test_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/changl/excel_api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4DF41D-8FC6-4C4C-A75E-4F97890BEA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BB47E4-02DF-AB4C-B697-0737DA730454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{FE8B6715-D06A-E049-99D2-C2B894523468}"/>
+    <workbookView xWindow="2100" yWindow="1840" windowWidth="28040" windowHeight="17440" xr2:uid="{FE8B6715-D06A-E049-99D2-C2B894523468}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>AUS</t>
   </si>
@@ -43,6 +43,18 @@
   </si>
   <si>
     <t>CHN</t>
+  </si>
+  <si>
+    <t>RUS</t>
+  </si>
+  <si>
+    <t>2021-08-11</t>
+  </si>
+  <si>
+    <t>2021-01-01</t>
+  </si>
+  <si>
+    <t>2011-08-01</t>
   </si>
 </sst>
 </file>
@@ -90,7 +102,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -406,33 +418,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC477003-1363-674F-9921-AA81DF974A38}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
-        <v>44418</v>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>44197</v>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>